<commit_message>
Minor corrections of column merging issues and column names
</commit_message>
<xml_diff>
--- a/Config/DatabaseInfo.xlsx
+++ b/Config/DatabaseInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\Data\SInAS workflow - native and alien\v10\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JLU-SU\Desktop\github update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5821DF-54DF-467B-A1D5-987B8AAA90DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6948A3F-5EC1-42C5-8812-A39A983F1C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22440" yWindow="1395" windowWidth="19770" windowHeight="12120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="75">
   <si>
     <t>Dataset_brief_name</t>
   </si>
@@ -94,75 +94,30 @@
     <t>Column_additional</t>
   </si>
   <si>
-    <t>MacroFungi</t>
-  </si>
-  <si>
-    <t>GlobalAlienMacroFungi_24Jun21.csv</t>
-  </si>
-  <si>
-    <t>Fungi</t>
-  </si>
-  <si>
     <t>scientificName</t>
   </si>
   <si>
     <t>kingdom</t>
   </si>
   <si>
-    <t>locality</t>
-  </si>
-  <si>
     <t>countryCode</t>
   </si>
   <si>
-    <t>year</t>
-  </si>
-  <si>
     <t>establishmentMeans</t>
   </si>
   <si>
-    <t>DAMA</t>
-  </si>
-  <si>
-    <t>Mammals</t>
-  </si>
-  <si>
     <t>Binomial</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>References</t>
-  </si>
-  <si>
-    <t>Pathway</t>
-  </si>
-  <si>
     <t>GRIIS</t>
   </si>
   <si>
-    <t>GRIIS - Country Compendium V1_0.csv</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
-    <t>recordID</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
-    <t>countryCode_alpha2</t>
-  </si>
-  <si>
-    <t>occurrenceStatus</t>
-  </si>
-  <si>
     <t>habitat</t>
   </si>
   <si>
@@ -190,9 +145,6 @@
     <t>FirstRecords</t>
   </si>
   <si>
-    <t>TaxonName</t>
-  </si>
-  <si>
     <t>FirstRecord</t>
   </si>
   <si>
@@ -283,129 +235,6 @@
     <t>Taxon</t>
   </si>
   <si>
-    <t>GlobalAlienSpeciesFirstRecordDatabase_v3.1_freedata.xlsx</t>
-  </si>
-  <si>
-    <t>InvasionStage</t>
-  </si>
-  <si>
-    <t>DAMA_AlienRegions.csv</t>
-  </si>
-  <si>
-    <t>ISO3</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>species</t>
-  </si>
-  <si>
-    <t>IUCN_Amph</t>
-  </si>
-  <si>
-    <t>Amphibians</t>
-  </si>
-  <si>
-    <t>sci_name</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>presence</t>
-  </si>
-  <si>
-    <t>Reptiles</t>
-  </si>
-  <si>
-    <t>IUCN_Mamm</t>
-  </si>
-  <si>
-    <t>BirdLife</t>
-  </si>
-  <si>
-    <t>origin</t>
-  </si>
-  <si>
-    <t>Plants</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t>Ants</t>
-  </si>
-  <si>
-    <t>GIATAR</t>
-  </si>
-  <si>
-    <t>FishBase</t>
-  </si>
-  <si>
-    <t>Fish</t>
-  </si>
-  <si>
-    <t>sisid</t>
-  </si>
-  <si>
-    <t>id_no</t>
-  </si>
-  <si>
-    <t>amphibians_IUCN_native.csv</t>
-  </si>
-  <si>
-    <t>birds_BirdLife_native.csv</t>
-  </si>
-  <si>
-    <t>reptiles_IUCN_native.csv</t>
-  </si>
-  <si>
-    <t>mammals_IUCN_native.csv</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>WoRMS</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>area_code_l3</t>
-  </si>
-  <si>
-    <t>ants_wong2023_native_alien.csv</t>
-  </si>
-  <si>
-    <t>fish_rfishbase_native_alien.csv</t>
-  </si>
-  <si>
-    <t>marine_worms_native_alien.csv</t>
-  </si>
-  <si>
-    <t>taxon_name</t>
-  </si>
-  <si>
-    <t>canonicalName</t>
-  </si>
-  <si>
-    <t>Ants_Wong</t>
-  </si>
-  <si>
-    <t>giatar_aliens_native.csv</t>
-  </si>
-  <si>
-    <t>plants_wcvp_native.csv</t>
-  </si>
-  <si>
-    <t>WCVP</t>
-  </si>
-  <si>
-    <t>IUCN_Rep</t>
-  </si>
-  <si>
     <t>Column_location</t>
   </si>
   <si>
@@ -413,6 +242,24 @@
   </si>
   <si>
     <t>Column_taxon</t>
+  </si>
+  <si>
+    <t>AmphibiansReptiles_Capinha-etal2017_example.xlsx</t>
+  </si>
+  <si>
+    <t>GAVIA_taxon_region_list_example.xlsx</t>
+  </si>
+  <si>
+    <t>GRIIS_sTwist_Hanno_Aug92019_resend_example.xlsx</t>
+  </si>
+  <si>
+    <t>GloNAF_taxon_region_list_example.xlsx</t>
+  </si>
+  <si>
+    <t>GlobalAlienSpeciesFirstRecordDatabase_v1.2_withcountries_example.xlsx</t>
+  </si>
+  <si>
+    <t>Author</t>
   </si>
 </sst>
 </file>
@@ -437,10 +284,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -466,20 +311,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{92CB3A98-F71C-40DD-9507-9E105B591987}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -757,11 +604,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S5" sqref="S5"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,7 +644,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -809,30 +656,30 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>123</v>
+        <v>66</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>124</v>
+        <v>67</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -844,65 +691,62 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" t="s">
-        <v>54</v>
-      </c>
       <c r="O2" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="P2" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="O3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="2" t="s">
+      <c r="R3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -911,405 +755,80 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
       <c r="I4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" t="s">
         <v>33</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="O5" t="s">
-        <v>27</v>
-      </c>
-      <c r="R5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
         <v>45</v>
       </c>
-      <c r="E6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" t="s">
-        <v>47</v>
+      <c r="K6" t="s">
+        <v>51</v>
       </c>
       <c r="M6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7" t="s">
-        <v>61</v>
-      </c>
-      <c r="O7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" t="s">
-        <v>61</v>
-      </c>
-      <c r="K8" t="s">
-        <v>67</v>
-      </c>
-      <c r="M8" t="s">
-        <v>68</v>
-      </c>
-      <c r="N8" t="s">
-        <v>69</v>
-      </c>
-      <c r="O8" t="s">
-        <v>69</v>
-      </c>
-      <c r="P8" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>117</v>
-      </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" t="s">
-        <v>86</v>
-      </c>
-      <c r="J9" t="s">
-        <v>85</v>
-      </c>
-      <c r="K9" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" t="s">
-        <v>68</v>
-      </c>
-      <c r="O9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" t="s">
-        <v>86</v>
-      </c>
-      <c r="M10" t="s">
-        <v>91</v>
-      </c>
-      <c r="N10" t="s">
-        <v>92</v>
-      </c>
-      <c r="O10" t="s">
-        <v>96</v>
-      </c>
-      <c r="R10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" t="s">
-        <v>90</v>
-      </c>
-      <c r="H11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" t="s">
-        <v>86</v>
-      </c>
-      <c r="M11" t="s">
-        <v>91</v>
-      </c>
-      <c r="N11" t="s">
-        <v>92</v>
-      </c>
-      <c r="O11" t="s">
-        <v>96</v>
-      </c>
-      <c r="R11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E12" t="s">
-        <v>90</v>
-      </c>
-      <c r="H12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" t="s">
-        <v>86</v>
-      </c>
-      <c r="M12" t="s">
-        <v>91</v>
-      </c>
-      <c r="N12" t="s">
-        <v>92</v>
-      </c>
-      <c r="O12" t="s">
-        <v>96</v>
-      </c>
-      <c r="R12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" t="s">
-        <v>103</v>
-      </c>
-      <c r="E13" t="s">
-        <v>90</v>
-      </c>
-      <c r="I13" t="s">
-        <v>86</v>
-      </c>
-      <c r="M13" t="s">
-        <v>91</v>
-      </c>
-      <c r="N13" t="s">
-        <v>92</v>
-      </c>
-      <c r="O13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" t="s">
-        <v>120</v>
-      </c>
-      <c r="C14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" t="s">
-        <v>116</v>
-      </c>
-      <c r="I14" t="s">
-        <v>98</v>
-      </c>
-      <c r="J14" t="s">
-        <v>112</v>
-      </c>
-      <c r="N14" t="s">
-        <v>41</v>
-      </c>
-      <c r="O14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>118</v>
-      </c>
-      <c r="B15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C15" t="s">
-        <v>99</v>
-      </c>
-      <c r="E15" t="s">
-        <v>87</v>
-      </c>
-      <c r="I15" t="s">
-        <v>75</v>
-      </c>
-      <c r="O15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" t="s">
-        <v>102</v>
-      </c>
-      <c r="E16" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" t="s">
-        <v>39</v>
-      </c>
-      <c r="O16" t="s">
-        <v>109</v>
-      </c>
-      <c r="R16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B17" t="s">
-        <v>115</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17" t="s">
-        <v>24</v>
-      </c>
-      <c r="O17" t="s">
-        <v>27</v>
+        <v>52</v>
+      </c>
+      <c r="N6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6" t="s">
+        <v>53</v>
+      </c>
+      <c r="P6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1412,20 +931,20 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="G2" s="2"/>
       <c r="I2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1525,159 +1044,159 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="S2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="K3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="M3" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="N3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="O3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="P3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="Q3" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" t="s">
-        <v>78</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="R4" t="s">
         <v>27</v>
       </c>
-      <c r="R4" t="s">
-        <v>42</v>
-      </c>
       <c r="S4" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="I5" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="O5" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" t="s">
         <v>37</v>
       </c>
-      <c r="E6" t="s">
-        <v>81</v>
-      </c>
-      <c r="I6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" t="s">
-        <v>52</v>
-      </c>
-      <c r="M6" t="s">
-        <v>53</v>
-      </c>
       <c r="N6" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="O6" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="P6" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="S6" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upload of full versions of input files
</commit_message>
<xml_diff>
--- a/Config/DatabaseInfo.xlsx
+++ b/Config/DatabaseInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\1. Data paper\SInAS-dataset_final_v2\SInAS-workflow_update\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\1. Data paper\SInAS_github\SInAS\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18687E8C-9558-4F0B-9D86-BCAD1CD06F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E515684-8DB9-4C7E-997E-DC6A1E78AB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="135">
   <si>
     <t>Dataset_brief_name</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t>native</t>
+  </si>
+  <si>
+    <t>citacion</t>
   </si>
 </sst>
 </file>
@@ -784,8 +787,8 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P6" sqref="P6"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1161,7 +1164,7 @@
         <v>86</v>
       </c>
       <c r="N10" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="O10" t="s">
         <v>92</v>
@@ -1199,7 +1202,7 @@
         <v>86</v>
       </c>
       <c r="N11" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="O11" t="s">
         <v>92</v>
@@ -1237,7 +1240,7 @@
         <v>86</v>
       </c>
       <c r="N12" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="O12" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
Upload of example versions of Input files and the corresponding configuration file with database information
</commit_message>
<xml_diff>
--- a/Config/DatabaseInfo.xlsx
+++ b/Config/DatabaseInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\1. Data paper\SInAS_github\SInAS\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JLU-SU\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C876D2F-9DC0-48C6-B528-A98D930048D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052F882F-D342-4CD8-B9EC-AD9DCF17575A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26190" yWindow="2595" windowWidth="23040" windowHeight="12120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27165" yWindow="2445" windowWidth="23040" windowHeight="12120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="87">
   <si>
     <t>Dataset_brief_name</t>
   </si>
@@ -94,75 +94,30 @@
     <t>Column_additional</t>
   </si>
   <si>
-    <t>MacroFungi</t>
-  </si>
-  <si>
-    <t>GlobalAlienMacroFungi_24Jun21.csv</t>
-  </si>
-  <si>
-    <t>Fungi</t>
-  </si>
-  <si>
     <t>scientificName</t>
   </si>
   <si>
     <t>kingdom</t>
   </si>
   <si>
-    <t>locality</t>
-  </si>
-  <si>
     <t>countryCode</t>
   </si>
   <si>
-    <t>year</t>
-  </si>
-  <si>
     <t>establishmentMeans</t>
   </si>
   <si>
-    <t>DAMA</t>
-  </si>
-  <si>
-    <t>Mammals</t>
-  </si>
-  <si>
     <t>Binomial</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>References</t>
-  </si>
-  <si>
-    <t>Pathway</t>
-  </si>
-  <si>
     <t>GRIIS</t>
   </si>
   <si>
-    <t>GRIIS - Country Compendium V1_0.csv</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
-    <t>recordID</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
-    <t>countryCode_alpha2</t>
-  </si>
-  <si>
-    <t>occurrenceStatus</t>
-  </si>
-  <si>
     <t>habitat</t>
   </si>
   <si>
@@ -190,9 +145,6 @@
     <t>FirstRecords</t>
   </si>
   <si>
-    <t>TaxonName</t>
-  </si>
-  <si>
     <t>FirstRecord</t>
   </si>
   <si>
@@ -283,163 +235,67 @@
     <t>Taxon</t>
   </si>
   <si>
-    <t>GlobalAlienSpeciesFirstRecordDatabase_v3.1_freedata.xlsx</t>
-  </si>
-  <si>
-    <t>InvasionStage</t>
-  </si>
-  <si>
-    <t>DAMA_AlienRegions.csv</t>
-  </si>
-  <si>
-    <t>ISO3</t>
+    <t>Column_location</t>
+  </si>
+  <si>
+    <t>Column_bibliographicCitation</t>
+  </si>
+  <si>
+    <t>Column_taxon</t>
+  </si>
+  <si>
+    <t>AmphibiansReptiles_Capinha-etal2017_example.xlsx</t>
+  </si>
+  <si>
+    <t>GAVIA_taxon_region_list_example.xlsx</t>
+  </si>
+  <si>
+    <t>GRIIS_sTwist_Hanno_Aug92019_resend_example.xlsx</t>
+  </si>
+  <si>
+    <t>GloNAF_taxon_region_list_example.xlsx</t>
+  </si>
+  <si>
+    <t>GlobalAlienSpeciesFirstRecordDatabase_v1.2_withcountries_example.xlsx</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Dataset_scope</t>
+  </si>
+  <si>
+    <t>alien</t>
+  </si>
+  <si>
+    <t>native</t>
+  </si>
+  <si>
+    <t>Amph_IUCN</t>
+  </si>
+  <si>
+    <t>Amphibians</t>
+  </si>
+  <si>
+    <t>id_no</t>
+  </si>
+  <si>
+    <t>sci_name</t>
   </si>
   <si>
     <t>location</t>
   </si>
   <si>
-    <t>species</t>
-  </si>
-  <si>
-    <t>IUCN_Amph</t>
-  </si>
-  <si>
-    <t>Amphibians</t>
-  </si>
-  <si>
-    <t>sci_name</t>
-  </si>
-  <si>
-    <t>source</t>
+    <t>citation</t>
   </si>
   <si>
     <t>presence</t>
   </si>
   <si>
-    <t>Reptiles</t>
-  </si>
-  <si>
-    <t>IUCN_Mamm</t>
-  </si>
-  <si>
-    <t>BirdLife</t>
-  </si>
-  <si>
     <t>origin</t>
   </si>
   <si>
-    <t>Plants</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t>Ants</t>
-  </si>
-  <si>
-    <t>GIATAR</t>
-  </si>
-  <si>
-    <t>FishBase</t>
-  </si>
-  <si>
-    <t>Fish</t>
-  </si>
-  <si>
-    <t>sisid</t>
-  </si>
-  <si>
-    <t>id_no</t>
-  </si>
-  <si>
-    <t>amphibians_IUCN_native.csv</t>
-  </si>
-  <si>
-    <t>birds_BirdLife_native.csv</t>
-  </si>
-  <si>
-    <t>reptiles_IUCN_native.csv</t>
-  </si>
-  <si>
-    <t>mammals_IUCN_native.csv</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>WoRMS</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>area_code_l3</t>
-  </si>
-  <si>
-    <t>ants_wong2023_native_alien.csv</t>
-  </si>
-  <si>
-    <t>fish_rfishbase_native_alien.csv</t>
-  </si>
-  <si>
-    <t>marine_worms_native_alien.csv</t>
-  </si>
-  <si>
-    <t>taxon_name</t>
-  </si>
-  <si>
-    <t>canonicalName</t>
-  </si>
-  <si>
-    <t>Ants_Wong</t>
-  </si>
-  <si>
-    <t>giatar_aliens_native.csv</t>
-  </si>
-  <si>
-    <t>plants_wcvp_native.csv</t>
-  </si>
-  <si>
-    <t>WCVP</t>
-  </si>
-  <si>
-    <t>IUCN_Rep</t>
-  </si>
-  <si>
-    <t>Column_location</t>
-  </si>
-  <si>
-    <t>Column_bibliographicCitation</t>
-  </si>
-  <si>
-    <t>Column_taxon</t>
-  </si>
-  <si>
-    <t>GloNAF_v3_taxon_region_reference.csv</t>
-  </si>
-  <si>
-    <t>taxon_corrected</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>reference</t>
-  </si>
-  <si>
-    <t>Dataset_scope</t>
-  </si>
-  <si>
-    <t>alien</t>
-  </si>
-  <si>
-    <t>alien; native</t>
-  </si>
-  <si>
-    <t>native</t>
-  </si>
-  <si>
-    <t>citation</t>
+    <t>amphibians_IUCN_native_example.csv</t>
   </si>
 </sst>
 </file>
@@ -464,10 +320,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -493,20 +347,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{92CB3A98-F71C-40DD-9507-9E105B591987}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -784,18 +640,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N10" sqref="N10"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5546875" customWidth="1"/>
     <col min="2" max="2" width="55.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="37.5546875" customWidth="1"/>
     <col min="4" max="6" width="18.33203125" customWidth="1"/>
     <col min="7" max="7" width="20.6640625" customWidth="1"/>
     <col min="8" max="8" width="13.21875" customWidth="1"/>
@@ -819,7 +675,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -828,7 +684,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -840,30 +696,30 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>123</v>
+        <v>66</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>124</v>
+        <v>67</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
@@ -875,68 +731,68 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" t="s">
-        <v>53</v>
-      </c>
       <c r="P2" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="Q2" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="I3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="P3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="2" t="s">
+      <c r="S3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -945,446 +801,126 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
       <c r="J4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" t="s">
         <v>33</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
-        <v>23</v>
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
       </c>
       <c r="J5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" t="s">
-        <v>40</v>
-      </c>
-      <c r="O5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="P5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>131</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s">
         <v>45</v>
       </c>
-      <c r="F6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" t="s">
-        <v>47</v>
+      <c r="L6" t="s">
+        <v>51</v>
       </c>
       <c r="N6" t="s">
-        <v>48</v>
+        <v>52</v>
+      </c>
+      <c r="O6" t="s">
+        <v>53</v>
+      </c>
+      <c r="P6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>53</v>
+      </c>
+      <c r="R6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>79</v>
+      </c>
+      <c r="E7" t="s">
+        <v>80</v>
       </c>
       <c r="F7" t="s">
-        <v>127</v>
+        <v>81</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
       </c>
       <c r="J7" t="s">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="N7" t="s">
-        <v>129</v>
+        <v>83</v>
+      </c>
+      <c r="O7" t="s">
+        <v>84</v>
       </c>
       <c r="P7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" t="s">
-        <v>67</v>
-      </c>
-      <c r="N8" t="s">
-        <v>68</v>
-      </c>
-      <c r="O8" t="s">
-        <v>69</v>
-      </c>
-      <c r="P8" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>69</v>
-      </c>
-      <c r="R8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C9" t="s">
-        <v>132</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" t="s">
-        <v>117</v>
-      </c>
-      <c r="G9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" t="s">
-        <v>86</v>
-      </c>
-      <c r="K9" t="s">
         <v>85</v>
       </c>
-      <c r="L9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N9" t="s">
-        <v>68</v>
-      </c>
-      <c r="P9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" t="s">
-        <v>133</v>
-      </c>
-      <c r="D10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" t="s">
-        <v>104</v>
-      </c>
-      <c r="F10" t="s">
-        <v>90</v>
-      </c>
-      <c r="I10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" t="s">
-        <v>86</v>
-      </c>
-      <c r="N10" t="s">
-        <v>134</v>
-      </c>
-      <c r="O10" t="s">
-        <v>92</v>
-      </c>
-      <c r="P10" t="s">
-        <v>96</v>
-      </c>
-      <c r="S10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" t="s">
-        <v>133</v>
-      </c>
-      <c r="D11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" t="s">
-        <v>90</v>
-      </c>
-      <c r="I11" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" t="s">
-        <v>86</v>
-      </c>
-      <c r="N11" t="s">
-        <v>134</v>
-      </c>
-      <c r="O11" t="s">
-        <v>92</v>
-      </c>
-      <c r="P11" t="s">
-        <v>96</v>
-      </c>
-      <c r="S11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" t="s">
-        <v>133</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" t="s">
-        <v>104</v>
-      </c>
-      <c r="F12" t="s">
-        <v>90</v>
-      </c>
-      <c r="I12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" t="s">
-        <v>86</v>
-      </c>
-      <c r="N12" t="s">
-        <v>134</v>
-      </c>
-      <c r="O12" t="s">
-        <v>92</v>
-      </c>
-      <c r="P12" t="s">
-        <v>96</v>
-      </c>
-      <c r="S12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C13" t="s">
-        <v>133</v>
-      </c>
-      <c r="D13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" t="s">
-        <v>90</v>
-      </c>
-      <c r="J13" t="s">
-        <v>86</v>
-      </c>
-      <c r="N13" t="s">
-        <v>91</v>
-      </c>
-      <c r="O13" t="s">
-        <v>92</v>
-      </c>
-      <c r="P13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" t="s">
-        <v>120</v>
-      </c>
-      <c r="C14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D14" t="s">
-        <v>97</v>
-      </c>
-      <c r="F14" t="s">
-        <v>116</v>
-      </c>
-      <c r="J14" t="s">
-        <v>98</v>
-      </c>
-      <c r="K14" t="s">
-        <v>112</v>
-      </c>
-      <c r="O14" t="s">
-        <v>41</v>
-      </c>
-      <c r="P14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>118</v>
-      </c>
-      <c r="B15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C15" t="s">
-        <v>132</v>
-      </c>
-      <c r="D15" t="s">
-        <v>99</v>
-      </c>
-      <c r="F15" t="s">
-        <v>87</v>
-      </c>
-      <c r="J15" t="s">
-        <v>75</v>
-      </c>
-      <c r="P15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" t="s">
-        <v>132</v>
-      </c>
-      <c r="D16" t="s">
-        <v>102</v>
-      </c>
-      <c r="F16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J16" t="s">
-        <v>39</v>
-      </c>
-      <c r="P16" t="s">
-        <v>109</v>
-      </c>
-      <c r="S16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B17" t="s">
-        <v>115</v>
-      </c>
-      <c r="C17" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" t="s">
-        <v>111</v>
-      </c>
-      <c r="F17" t="s">
-        <v>87</v>
-      </c>
-      <c r="J17" t="s">
-        <v>24</v>
-      </c>
-      <c r="P17" t="s">
+      <c r="S7" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1488,20 +1024,20 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="G2" s="2"/>
       <c r="I2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1601,159 +1137,159 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="S2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="K3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="M3" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="N3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="O3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="P3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="Q3" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" t="s">
-        <v>78</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="R4" t="s">
         <v>27</v>
       </c>
-      <c r="R4" t="s">
-        <v>42</v>
-      </c>
       <c r="S4" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="I5" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="O5" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" t="s">
         <v>37</v>
       </c>
-      <c r="E6" t="s">
-        <v>81</v>
-      </c>
-      <c r="I6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" t="s">
-        <v>52</v>
-      </c>
-      <c r="M6" t="s">
-        <v>53</v>
-      </c>
       <c r="N6" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="O6" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="P6" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="S6" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update SInAS_Workflow_Manual and color formatting of DatabaseInfo
</commit_message>
<xml_diff>
--- a/Config/DatabaseInfo.xlsx
+++ b/Config/DatabaseInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JLU-SU\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\1. Data paper\SInAS_github\SInAS\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052F882F-D342-4CD8-B9EC-AD9DCF17575A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682DDD36-00EC-47F1-B863-0C048FB2AD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27165" yWindow="2445" windowWidth="23040" windowHeight="12120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -324,18 +324,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -357,8 +351,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,8 +637,8 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B8" sqref="B8"/>
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,65 +661,65 @@
     <col min="20" max="20" width="34.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -745,7 +739,7 @@
       <c r="F2" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>74</v>
       </c>
       <c r="J2" t="s">

</xml_diff>

<commit_message>
Minor correction of filling of bibliographic citations and handling of event dates
</commit_message>
<xml_diff>
--- a/Config/DatabaseInfo.xlsx
+++ b/Config/DatabaseInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\1. Data paper\SInAS_github\SInAS\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682DDD36-00EC-47F1-B863-0C048FB2AD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D74AA38-30E1-4B4F-A66C-E3D32A50A198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="92">
   <si>
     <t>Dataset_brief_name</t>
   </si>
@@ -286,9 +286,6 @@
     <t>location</t>
   </si>
   <si>
-    <t>citation</t>
-  </si>
-  <si>
     <t>presence</t>
   </si>
   <si>
@@ -296,6 +293,24 @@
   </si>
   <si>
     <t>amphibians_IUCN_native_example.csv</t>
+  </si>
+  <si>
+    <t>Seebens, H. et al. No saturation in the accumulation of alien species worldwide. Nat. Commun. 8, 14435 (2017)</t>
+  </si>
+  <si>
+    <t>Pagad, S. et al. Country Compendium of the Global Register of Introduced and Invasive Species. Sci. Data 9, 391 (2022)</t>
+  </si>
+  <si>
+    <t>Capinha, C. et al. Diversity, biogeography and the global flows of alien amphibians and reptiles. Divers. Distrib. 23, 1313–1322 (2017)</t>
+  </si>
+  <si>
+    <t>van Kleunen, M. et al. The Global Naturalized Alien Flora (GloNAF) database. Ecology 100, e02542 (2019)</t>
+  </si>
+  <si>
+    <t>Dyer, E. E., Redding, D. W. &amp; Blackburn, T. M. The global avian invasions atlas, a database of alien bird distributions worldwide. Sci. Data 4, 170041 (2017)</t>
+  </si>
+  <si>
+    <t>IUCN. The IUCN Red List of Threatened Species. https://www.iucnredlist.org (2025)</t>
   </si>
 </sst>
 </file>
@@ -345,14 +360,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,8 +651,8 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K5" sqref="K5"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -661,65 +675,65 @@
     <col min="20" max="20" width="34.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -749,7 +763,7 @@
         <v>36</v>
       </c>
       <c r="N2" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="P2" t="s">
         <v>38</v>
@@ -783,6 +797,9 @@
       <c r="K3" t="s">
         <v>21</v>
       </c>
+      <c r="N3" t="s">
+        <v>87</v>
+      </c>
       <c r="P3" t="s">
         <v>22</v>
       </c>
@@ -810,7 +827,7 @@
         <v>32</v>
       </c>
       <c r="N4" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -835,6 +852,9 @@
       <c r="J5" t="s">
         <v>45</v>
       </c>
+      <c r="N5" t="s">
+        <v>89</v>
+      </c>
       <c r="P5" t="s">
         <v>46</v>
       </c>
@@ -865,7 +885,7 @@
         <v>51</v>
       </c>
       <c r="N6" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="O6" t="s">
         <v>53</v>
@@ -885,7 +905,7 @@
         <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
         <v>77</v>
@@ -906,13 +926,13 @@
         <v>82</v>
       </c>
       <c r="N7" t="s">
+        <v>91</v>
+      </c>
+      <c r="O7" t="s">
         <v>83</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>84</v>
-      </c>
-      <c r="P7" t="s">
-        <v>85</v>
       </c>
       <c r="S7" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Update of SInAS version name and of bibliographic citations to data sources
</commit_message>
<xml_diff>
--- a/Config/DatabaseInfo.xlsx
+++ b/Config/DatabaseInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\1. Data paper\SInAS_github\SInAS\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D74AA38-30E1-4B4F-A66C-E3D32A50A198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7594C5-4626-4683-8EE1-01CDA2D20602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -295,29 +295,29 @@
     <t>amphibians_IUCN_native_example.csv</t>
   </si>
   <si>
-    <t>Seebens, H. et al. No saturation in the accumulation of alien species worldwide. Nat. Commun. 8, 14435 (2017)</t>
-  </si>
-  <si>
-    <t>Pagad, S. et al. Country Compendium of the Global Register of Introduced and Invasive Species. Sci. Data 9, 391 (2022)</t>
-  </si>
-  <si>
     <t>Capinha, C. et al. Diversity, biogeography and the global flows of alien amphibians and reptiles. Divers. Distrib. 23, 1313–1322 (2017)</t>
   </si>
   <si>
-    <t>van Kleunen, M. et al. The Global Naturalized Alien Flora (GloNAF) database. Ecology 100, e02542 (2019)</t>
-  </si>
-  <si>
-    <t>Dyer, E. E., Redding, D. W. &amp; Blackburn, T. M. The global avian invasions atlas, a database of alien bird distributions worldwide. Sci. Data 4, 170041 (2017)</t>
-  </si>
-  <si>
-    <t>IUCN. The IUCN Red List of Threatened Species. https://www.iucnredlist.org (2025)</t>
+    <t>Seebens, H. Alien Species First Records Database. Zenodo https://doi.org/10.5281/ZENODO.10039630 (2023) (v. 3.1)</t>
+  </si>
+  <si>
+    <t>Shyama Pagad, Bisset, S. &amp; McGeoch, M. A. Country Compendium of the Global Register of Introduced and Invasive Species. Dataset. Zenodo https://doi.org/10.5281/ZENODO.6348164 (2022)</t>
+  </si>
+  <si>
+    <t>Davis, A. J. S. et al. Global Naturalized Alien Flora (GloNAF). Open access data to support research on understanding global plant invasions. Zenodo https://doi.org/10.5281/ZENODO.17105725 (2025) (v. 3)</t>
+  </si>
+  <si>
+    <t>Dyer, E., Redding, D. &amp; Blackburn, T. Data from: The Global Avian Invasions Atlas - A database of alien bird distributions worldwide. Figshare https://doi.org/10.6084/M9.FIGSHARE.4234850.V1 (2016)</t>
+  </si>
+  <si>
+    <t>IUCN. The IUCN Red List of Threatened Species. https://www.iucnredlist.org (v. 2024-2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -337,6 +337,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -360,13 +367,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,8 +659,8 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N7" sqref="N7"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +674,8 @@
     <col min="9" max="9" width="15.33203125" customWidth="1"/>
     <col min="10" max="10" width="15.21875" customWidth="1"/>
     <col min="11" max="11" width="18.109375" customWidth="1"/>
-    <col min="12" max="14" width="18.6640625" customWidth="1"/>
+    <col min="12" max="13" width="18.6640625" customWidth="1"/>
+    <col min="14" max="14" width="94" customWidth="1"/>
     <col min="15" max="15" width="15.109375" customWidth="1"/>
     <col min="16" max="16" width="18.6640625" customWidth="1"/>
     <col min="17" max="17" width="13.6640625" customWidth="1"/>
@@ -762,8 +771,8 @@
       <c r="L2" t="s">
         <v>36</v>
       </c>
-      <c r="N2" t="s">
-        <v>86</v>
+      <c r="N2" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="P2" t="s">
         <v>38</v>
@@ -797,8 +806,8 @@
       <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="N3" t="s">
-        <v>87</v>
+      <c r="N3" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="P3" t="s">
         <v>22</v>
@@ -827,7 +836,7 @@
         <v>32</v>
       </c>
       <c r="N4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -852,7 +861,7 @@
       <c r="J5" t="s">
         <v>45</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="4" t="s">
         <v>89</v>
       </c>
       <c r="P5" t="s">
@@ -884,7 +893,7 @@
       <c r="L6" t="s">
         <v>51</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="4" t="s">
         <v>90</v>
       </c>
       <c r="O6" t="s">
@@ -925,7 +934,7 @@
       <c r="J7" t="s">
         <v>82</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="4" t="s">
         <v>91</v>
       </c>
       <c r="O7" t="s">

</xml_diff>